<commit_message>
renormalize all file, and make all file with ln new line
</commit_message>
<xml_diff>
--- a/Python/dokumentasi saya/transaksi.xlsx
+++ b/Python/dokumentasi saya/transaksi.xlsx
@@ -1,27 +1,3 @@
-
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiexin\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24975" windowHeight="10155"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
-</workbook>
-</file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">

</xml_diff>